<commit_message>
BATRU validator + SANOFIUA template fix
</commit_message>
<xml_diff>
--- a/Projects/SANOFIUA/Data/Template.xlsx
+++ b/Projects/SANOFIUA/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,12 +16,12 @@
     <sheet name="Primary&amp;Secondary_Facings" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$I$2:$J$16</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$16</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$H$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$I$2:$J$16</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$I$2:$J$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">MSL!$I$2:$J$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
@@ -39,6 +39,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$H$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$G$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'primary shelf_location'!#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'primary shelf_location'!#ref!</definedName>
@@ -68,26 +69,27 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$25</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$25</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -114,18 +116,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Solomon, Bonver /AE/EXT:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>to confirm what skus are included on brand block</t>
+          <t xml:space="preserve">Solomon, Bonver /AE/EXT:
+to confirm what skus are included on brand block</t>
         </r>
       </text>
     </comment>
@@ -149,18 +141,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Solomon, Bonver /AE/EXT:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>to confirm what skus are included on brand block</t>
+          <t xml:space="preserve">Solomon, Bonver /AE/EXT:
+to confirm what skus are included on brand block</t>
         </r>
       </text>
     </comment>
@@ -169,361 +151,355 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="115">
   <si>
-    <t>KPI Name</t>
+    <t xml:space="preserve">KPI Name</t>
   </si>
   <si>
-    <t>KPI Group</t>
+    <t xml:space="preserve">KPI Group</t>
   </si>
   <si>
-    <t>KPI Type</t>
+    <t xml:space="preserve">KPI Type</t>
   </si>
   <si>
-    <t>Tested Group</t>
+    <t xml:space="preserve">Tested Group</t>
   </si>
   <si>
-    <t>Template Group</t>
+    <t xml:space="preserve">Template Group</t>
   </si>
   <si>
-    <t>Sheet</t>
+    <t xml:space="preserve">Sheet</t>
   </si>
   <si>
-    <t>SCORE</t>
+    <t xml:space="preserve">SCORE</t>
   </si>
   <si>
-    <t>Shelf Location Compliance</t>
+    <t xml:space="preserve">Shelf Location Compliance</t>
   </si>
   <si>
-    <t>Primary Shelf</t>
+    <t xml:space="preserve">Primary Shelf</t>
   </si>
   <si>
-    <t>Shelf Level Per Brand</t>
+    <t xml:space="preserve">Shelf Level Per Brand</t>
   </si>
   <si>
-    <t>Primary Shelf_Location</t>
+    <t xml:space="preserve">Primary Shelf_Location</t>
   </si>
   <si>
-    <t>numeric</t>
+    <t xml:space="preserve">numeric</t>
   </si>
   <si>
-    <t>POSM Availability Primary</t>
+    <t xml:space="preserve">POSM Availability Primary</t>
   </si>
   <si>
-    <t>Product Availability Per SKU</t>
+    <t xml:space="preserve">Product Availability Per SKU</t>
   </si>
   <si>
-    <t>Primary&amp;Secondary_POSM</t>
+    <t xml:space="preserve">Primary&amp;Secondary_POSM</t>
   </si>
   <si>
-    <t>Product Minimum Facings Primary</t>
+    <t xml:space="preserve">Product Minimum Facings Primary</t>
   </si>
   <si>
-    <t>Primary&amp;Secondary_Facings</t>
+    <t xml:space="preserve">Primary&amp;Secondary_Facings</t>
   </si>
   <si>
-    <t>Product Minimum Facings Secondary</t>
+    <t xml:space="preserve">Product Minimum Facings Secondary</t>
   </si>
   <si>
-    <t>Secondary Shelf</t>
+    <t xml:space="preserve">Secondary Shelf</t>
   </si>
   <si>
-    <t>Blocked Together</t>
+    <t xml:space="preserve">Blocked Together</t>
   </si>
   <si>
-    <t>Blocked Together Per Brand</t>
+    <t xml:space="preserve">Blocked Together Per Brand</t>
   </si>
   <si>
-    <t>Primary_Brand_Blocking</t>
+    <t xml:space="preserve">Primary_Brand_Blocking</t>
   </si>
   <si>
-    <t>POSM Availability Secondary</t>
+    <t xml:space="preserve">POSM Availability Secondary</t>
   </si>
   <si>
-    <t>MSL Compliance</t>
+    <t xml:space="preserve">MSL Compliance</t>
   </si>
   <si>
-    <t>MSL</t>
+    <t xml:space="preserve">MSL</t>
   </si>
   <si>
-    <t>Perfect Store</t>
+    <t xml:space="preserve">Perfect Store</t>
   </si>
   <si>
-    <t>Primary Shelf Compliance</t>
+    <t xml:space="preserve">Primary Shelf Compliance</t>
   </si>
   <si>
-    <t>Secondary Shelf Compliance</t>
+    <t xml:space="preserve">Secondary Shelf Compliance</t>
   </si>
   <si>
-    <t>Perfect Store Compliance</t>
+    <t xml:space="preserve">Perfect Store Compliance</t>
   </si>
   <si>
-    <t>Sum of KPIs in Group</t>
+    <t xml:space="preserve">Sum of KPIs in Group</t>
   </si>
   <si>
-    <t>store type</t>
+    <t xml:space="preserve">store type</t>
   </si>
   <si>
-    <t>Product Name</t>
+    <t xml:space="preserve">Product Name</t>
   </si>
   <si>
-    <t>Product EAN Code</t>
+    <t xml:space="preserve">Product EAN Code</t>
   </si>
   <si>
-    <t>Brand</t>
+    <t xml:space="preserve">Brand</t>
   </si>
   <si>
-    <t>Category</t>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
-    <t>Points</t>
+    <t xml:space="preserve">Points</t>
   </si>
   <si>
-    <t>Non-Contracted</t>
+    <t xml:space="preserve">Non-Contracted</t>
   </si>
   <si>
-    <t>Contracted A</t>
+    <t xml:space="preserve">Contracted A</t>
   </si>
   <si>
-    <t>Contracted B</t>
+    <t xml:space="preserve">Contracted B</t>
   </si>
   <si>
-    <t>Contracted C</t>
+    <t xml:space="preserve">Contracted C</t>
   </si>
   <si>
-    <t>Essentiale forte N caps №30</t>
+    <t xml:space="preserve">Essentiale forte N caps №30</t>
   </si>
   <si>
-    <t>Essetiale</t>
+    <t xml:space="preserve">Essetiale</t>
   </si>
   <si>
-    <t>DH</t>
+    <t xml:space="preserve">DH</t>
   </si>
   <si>
-    <t>Festal Neo 10 000  tabs №20</t>
+    <t xml:space="preserve">Festal Neo 10 000  tabs №20</t>
   </si>
   <si>
-    <t>Festal </t>
+    <t xml:space="preserve">Festal </t>
   </si>
   <si>
-    <t>Enterogermina oral susp. 5 ml, vial №10</t>
+    <t xml:space="preserve">Enterogermina oral susp. 5 ml, vial №10</t>
   </si>
   <si>
-    <t>Enterogermina</t>
+    <t xml:space="preserve">Enterogermina</t>
   </si>
   <si>
-    <t>Enterogermina forte oral susp. 5 ml, vial №10</t>
+    <t xml:space="preserve">Enterogermina forte oral susp. 5 ml, vial №10</t>
   </si>
   <si>
-    <t>Maalox 2DC tabs №40</t>
+    <t xml:space="preserve">Maalox 2DC tabs №40</t>
   </si>
   <si>
-    <t>Maalox</t>
+    <t xml:space="preserve">Maalox</t>
   </si>
   <si>
-    <t>Maalox susp. 15 ml, sach. №30</t>
+    <t xml:space="preserve">Maalox susp. 15 ml, sach. №30</t>
   </si>
   <si>
-    <t>Lasolvan® Syrup 15mg/5ml 100ml woodb.№1</t>
+    <t xml:space="preserve">Lasolvan® Syrup 15mg/5ml 100ml woodb.№1</t>
   </si>
   <si>
-    <t>Lasolvan</t>
+    <t xml:space="preserve">Lasolvan</t>
   </si>
   <si>
-    <t>Cough </t>
+    <t xml:space="preserve">Cough </t>
   </si>
   <si>
-    <t>Lasolvan® strawb. syrup 100 ml (30 mg/ 5 ml), bottle №1</t>
+    <t xml:space="preserve">Lasolvan® strawb. syrup 100 ml (30 mg/ 5 ml), bottle №1</t>
   </si>
   <si>
-    <t>Lasolvan® tablets 30mg, blist.№50(10х5)</t>
+    <t xml:space="preserve">Lasolvan® tablets 30mg, blist.№50(10х5)</t>
   </si>
   <si>
-    <t>Pinosol nasal drops 10 ml, vial №1</t>
+    <t xml:space="preserve">Pinosol nasal drops 10 ml, vial №1</t>
   </si>
   <si>
-    <t>Pinosol</t>
+    <t xml:space="preserve">Pinosol</t>
   </si>
   <si>
-    <t>Magne-B6 tabs №50</t>
+    <t xml:space="preserve">Magne-B6 tabs №50</t>
   </si>
   <si>
-    <t>Magne B6</t>
+    <t xml:space="preserve">Magne B6</t>
   </si>
   <si>
-    <t>VMS</t>
+    <t xml:space="preserve">VMS</t>
   </si>
   <si>
-    <t>Magne-B6 Antistress tabs #60</t>
+    <t xml:space="preserve">Magne-B6 Antistress tabs #60</t>
   </si>
   <si>
-    <t>No-spa tabs 40 mg №24</t>
+    <t xml:space="preserve">No-spa tabs 40 mg №24</t>
   </si>
   <si>
-    <t>NoSpa</t>
+    <t xml:space="preserve">NoSpa</t>
   </si>
   <si>
-    <t>Pain</t>
+    <t xml:space="preserve">Pain</t>
   </si>
   <si>
-    <t>No-spa tabs 40 mg №100</t>
+    <t xml:space="preserve">No-spa tabs 40 mg №100</t>
   </si>
   <si>
-    <t>SKUs</t>
+    <t xml:space="preserve">SKUs</t>
   </si>
   <si>
-    <t>Enterogermina caps № 12</t>
+    <t xml:space="preserve">Enterogermina caps № 12</t>
   </si>
   <si>
-    <t>Maalox susp. 250 ml, bottle №1</t>
+    <t xml:space="preserve">Maalox susp. 250 ml, bottle №1</t>
   </si>
   <si>
-    <t>Pinosol nasal spray 10 ml, vial №1</t>
+    <t xml:space="preserve">Pinosol nasal spray 10 ml, vial №1</t>
   </si>
   <si>
-    <t>Magne-B6 oral sol. 10 ml, amp. №10</t>
+    <t xml:space="preserve">Magne-B6 oral sol. 10 ml, amp. №10</t>
   </si>
   <si>
-    <t>No-spa Comfort tabs 40 mg №24</t>
+    <t xml:space="preserve">No-spa Comfort tabs 40 mg №24</t>
   </si>
   <si>
-    <t>No-spa tabs 40 mg №60</t>
+    <t xml:space="preserve">No-spa tabs 40 mg №60</t>
   </si>
   <si>
-    <t>No-spa forte tabs 80 mg №24</t>
+    <t xml:space="preserve">No-spa forte tabs 80 mg №24</t>
   </si>
   <si>
-    <t>Lasolvan® MAX caps 75 mg №10</t>
+    <t xml:space="preserve">Lasolvan® MAX caps 75 mg №10</t>
   </si>
   <si>
-    <t>Lasolvan® woodb. syrup 200 ml (15 mg/ 5 ml), bottle №1</t>
+    <t xml:space="preserve">Lasolvan® woodb. syrup 200 ml (15 mg/ 5 ml), bottle №1</t>
   </si>
   <si>
-    <t>Ignore empty</t>
+    <t xml:space="preserve">Ignore empty</t>
   </si>
   <si>
-    <t>Enterogermina oral susp. 5 ml, vial №10, Enterogermina forte oral susp. 5 ml, vial №10, Enterogermina caps № 12</t>
+    <t xml:space="preserve">Enterogermina oral susp. 5 ml, vial №10, Enterogermina forte oral susp. 5 ml, vial №10, Enterogermina caps № 12</t>
   </si>
   <si>
-    <t>3582910022428, 3582910078357, 3582910054894</t>
+    <t xml:space="preserve">3582910022428, 3582910078357, 3582910054894</t>
   </si>
   <si>
-    <t>Magne-B6 tabs №50, Magne-B6 Antistress tabs #60, Magne-B6 oral sol. 10 ml, amp. №10</t>
+    <t xml:space="preserve">Magne-B6 tabs №50, Magne-B6 Antistress tabs #60, Magne-B6 oral sol. 10 ml, amp. №10</t>
   </si>
   <si>
-    <t>3582910071440, 3582910071464, 3582910019428</t>
+    <t xml:space="preserve">3582910071440, 3582910071464, 3582910019428</t>
   </si>
   <si>
-    <t>No-spa tabs 40 mg №24, No-spa tabs 40 mg №100, No-spa Comfort tabs 40 mg №24, No-spa forte tabs 80 mg №24,No-spa tabs 40 mg №60</t>
+    <t xml:space="preserve">No-spa tabs 40 mg №24, No-spa tabs 40 mg №100, No-spa Comfort tabs 40 mg №24, No-spa forte tabs 80 mg №24,No-spa tabs 40 mg №60</t>
   </si>
   <si>
-    <t>3582910061557, 5997086103280, 3582910078326, 3582910066958, 5997086105055</t>
+    <t xml:space="preserve">3582910061557, 5997086103280, 3582910078326, 3582910066958, 5997086105055</t>
   </si>
   <si>
-    <t>Lasolvan® strawb. syrup 100 ml (30 mg/ 5 ml), bottle №1,Lasolvan® woodb. syrup 100 ml (15 mg/ 5 ml), bottle №1,Lasolvan® tablets 30mg, blist.№50(10х5), Lasolvan® MAX caps 75 mg №10Lasolvan® strawb. syrup 100 ml (30 mg/ 5 ml), bottle №1</t>
+    <t xml:space="preserve">Lasolvan® strawb. syrup 100 ml (30 mg/ 5 ml), bottle №1,Lasolvan® woodb. syrup 100 ml (15 mg/ 5 ml), bottle №1,Lasolvan® tablets 30mg, blist.№50(10х5), Lasolvan® MAX caps 75 mg №10Lasolvan® strawb. syrup 100 ml (30 mg/ 5 ml), bottle №1</t>
   </si>
   <si>
-    <t>9006968005935, 9006968005911, 9006968002156, 9006968010373, 9006968005935</t>
+    <t xml:space="preserve">9006968005935, 9006968005911, 9006968002156, 9006968010373, 9006968005935</t>
   </si>
   <si>
-    <t>UK Enterogermina Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK Enterogermina Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-CC-01</t>
+    <t xml:space="preserve">UK-CC-01</t>
   </si>
   <si>
-    <t>UK Maalox Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK Maalox Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-STS-02</t>
+    <t xml:space="preserve">UK-STS-02</t>
   </si>
   <si>
-    <t>UK NoSpa Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK NoSpa Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-STS-03</t>
+    <t xml:space="preserve">UK-STS-03</t>
   </si>
   <si>
-    <t>UK Festal Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK Festal Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-STS-04</t>
+    <t xml:space="preserve">UK-STS-04</t>
   </si>
   <si>
-    <t>Festal</t>
+    <t xml:space="preserve">Festal</t>
   </si>
   <si>
-    <t>UK Magne B6 Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK Magne B6 Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-STS-05</t>
+    <t xml:space="preserve">UK-STS-05</t>
   </si>
   <si>
-    <t>UK Pinosol Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK Pinosol Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-STS-06</t>
+    <t xml:space="preserve">UK-STS-06</t>
   </si>
   <si>
-    <t>Pinosol </t>
+    <t xml:space="preserve">Pinosol </t>
   </si>
   <si>
-    <t>C&amp;C</t>
+    <t xml:space="preserve">C&amp;C</t>
   </si>
   <si>
-    <t>UK Lasolvan Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK Lasolvan Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-STS-07</t>
+    <t xml:space="preserve">UK-STS-07</t>
   </si>
   <si>
-    <t>UK Essentiale Shelf Talker/Strip</t>
+    <t xml:space="preserve">UK Essentiale Shelf Talker/Strip</t>
   </si>
   <si>
-    <t>UK-STS-08</t>
+    <t xml:space="preserve">UK-STS-08</t>
   </si>
   <si>
-    <t>Essentiale </t>
+    <t xml:space="preserve">Essentiale </t>
   </si>
   <si>
-    <t>UK NoSpa product dispenser</t>
+    <t xml:space="preserve">UK NoSpa product dispenser</t>
   </si>
   <si>
-    <t>UK-PD-01</t>
+    <t xml:space="preserve">UK-PD-01</t>
   </si>
   <si>
-    <t>UK NoSpa product poster with
+    <t xml:space="preserve">UK NoSpa product poster with
 Shopper promo communication</t>
   </si>
   <si>
-    <t>UK-PD-02</t>
+    <t xml:space="preserve">UK-PD-02</t>
   </si>
   <si>
-    <t>UK Essentiale Shelf Talker/Strip poster with
+    <t xml:space="preserve">UK Essentiale Shelf Talker/Strip poster with
 Shopper promo communication</t>
   </si>
   <si>
-    <t>UK-STS-09</t>
-  </si>
-  <si>
-    <t>UK Festal Shelf Talker/Strip poster with
+    <t xml:space="preserve">UK Festal Shelf Talker/Strip poster with
 Shopper promo communication</t>
   </si>
   <si>
-    <t>UK-STS-10</t>
-  </si>
-  <si>
-    <t>UK Enterogermina Shelf Talker/Strip poster with
+    <t xml:space="preserve">UK Enterogermina Shelf Talker/Strip poster with
 Shopper promo communication</t>
   </si>
   <si>
-    <t>UK-CC-02</t>
+    <t xml:space="preserve">UK-STS-01</t>
   </si>
   <si>
-    <t>Magne B7</t>
+    <t xml:space="preserve">Magne B7</t>
   </si>
   <si>
-    <t> No-spa tabs 40 mg №24</t>
+    <t xml:space="preserve"> No-spa tabs 40 mg №24</t>
   </si>
 </sst>
 </file>
@@ -531,14 +507,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0000"/>
     <numFmt numFmtId="168" formatCode="0"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* \-??\ _₽_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -659,13 +635,6 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1308,35 +1277,79 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="6" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="6" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="6" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="8" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="19" fillId="8" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="8" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="8" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="23" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="6" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1344,75 +1357,31 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="9" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="9" borderId="23" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="6" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="22" fillId="2" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="22" fillId="2" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="9" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="2" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="23" fillId="2" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="24" fillId="12" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="23" fillId="12" borderId="5" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1510,13 +1479,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.0647773279352"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.748987854251"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2024291497976"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9716599190283"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.9473684210526"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.2024291497976"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,17 +1749,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="49.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="21" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="21" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="21" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="21" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="14.3238866396761"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="51.0445344129555"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="25.0931174089069"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="10.7773279352227"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="17.3805668016194"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="21" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="21" width="14.9311740890688"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="21" width="16.6477732793522"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="21" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6316,7 +6285,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="I2:J16"/>
+  <autoFilter ref="A2:H16"/>
   <mergeCells count="1">
     <mergeCell ref="G1:J1"/>
   </mergeCells>
@@ -6345,14 +6314,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="21" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="23.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="44.0769230769231"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="21.0607287449393"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="17.3805668016194"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="21" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7046,17 +7015,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="60" width="62.4493927125506"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="21" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="21" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="1023" min="11" style="21" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="14.8097165991903"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="21" width="11.2631578947368"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="60" width="64.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="21" width="26.9311740890688"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="21" width="17.3805668016194"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="21" width="14.8097165991903"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="21" width="10.7773279352227"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="21" width="12.3603238866397"/>
+    <col collapsed="false" hidden="false" max="1023" min="11" style="21" width="9.54655870445344"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11382,22 +11351,21 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="77" width="24.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="77" width="37.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="77" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="77" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="77" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="77" width="14.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="77" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="77" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="77" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="77" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="77" width="24.9716599190283"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="77" width="38.8056680161943"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="77" width="22.7651821862348"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="77" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="77" width="11.2631578947368"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="77" width="14.8097165991903"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="77" width="14.9311740890688"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="77" width="16.1619433198381"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="77" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11732,7 +11700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="90" t="s">
         <v>22</v>
       </c>
@@ -11740,7 +11708,7 @@
         <v>109</v>
       </c>
       <c r="C13" s="86" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D13" s="86" t="s">
         <v>104</v>
@@ -11761,15 +11729,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="90" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="86" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" s="86" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D14" s="86" t="s">
         <v>93</v>
@@ -11790,15 +11758,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="90" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="86" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C15" s="91" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D15" s="86" t="s">
         <v>46</v>
@@ -11841,23 +11809,23 @@
   </sheetPr>
   <dimension ref="1:29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="77" width="29.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="77" width="49.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="77" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="77" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="77" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="77" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="77" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="77" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="77" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="77" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="77" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="77" width="29.8704453441296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="77" width="51.0445344129555"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="77" width="25.0931174089069"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="77" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="77" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="77" width="10.7773279352227"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="77" width="17.3805668016194"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="77" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="77" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="77" width="19.9514170040486"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="77" width="9.54655870445344"/>
   </cols>
   <sheetData>
     <row r="1" s="93" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15108,7 +15076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="96" t="s">
         <v>15</v>
       </c>
@@ -15116,7 +15084,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="98" t="n">
-        <v>3582910071242</v>
+        <v>3587080002768</v>
       </c>
       <c r="D8" s="97" t="s">
         <v>49</v>
@@ -15311,7 +15279,7 @@
         <v>3582910019428</v>
       </c>
       <c r="D14" s="97" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E14" s="97" t="s">
         <v>60</v>
@@ -15332,7 +15300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="96" t="s">
         <v>15</v>
       </c>
@@ -15340,7 +15308,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="98" t="n">
-        <v>3582910071464</v>
+        <v>3582910026334</v>
       </c>
       <c r="D15" s="97" t="s">
         <v>59</v>
@@ -15364,7 +15332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="96" t="s">
         <v>15</v>
       </c>
@@ -15372,7 +15340,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="98" t="n">
-        <v>5997086105055</v>
+        <v>5997086705055</v>
       </c>
       <c r="D16" s="97" t="s">
         <v>63</v>
@@ -15785,7 +15753,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="102" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C29" s="103" t="n">
         <v>3582910061557</v>
@@ -15813,7 +15781,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G25"/>
+  <autoFilter ref="A2:H25"/>
   <mergeCells count="1">
     <mergeCell ref="G1:J1"/>
   </mergeCells>

</xml_diff>